<commit_message>
commit the code upto 19/06/2025
</commit_message>
<xml_diff>
--- a/demoproject/src/test/resources/testdata.xlsx
+++ b/demoproject/src/test/resources/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D E L L\git\DemoProject\demoproject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E9681-9016-4F35-B2A3-37BE82422822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFD9D91-12E9-49AD-BB20-4A2EAAE06079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="2430" windowWidth="15375" windowHeight="7875" xr2:uid="{5316CAC7-B33A-47ED-A611-1D53E5F18C0D}"/>
+    <workbookView xWindow="3885" yWindow="2160" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{5316CAC7-B33A-47ED-A611-1D53E5F18C0D}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
     <sheet name="managenews" sheetId="2" r:id="rId2"/>
+    <sheet name="adminusers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>pasww</t>
+  </si>
+  <si>
+    <t>UsernamePassword</t>
+  </si>
+  <si>
+    <t>pbv</t>
   </si>
 </sst>
 </file>
@@ -403,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60565011-5F85-4382-BB8B-72B8FF7478A3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -484,4 +491,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8E8E53-0D4E-4664-A119-60B820E52135}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>